<commit_message>
assignment #2 amelia -> eddie
added two figs, all data already clean
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2ECruz.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2ECruz.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{07CE8D1E-4D55-4D43-B812-8FF8CB8AA451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{530887C6-E125-4069-8436-DAA17B42DCD4}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{07CE8D1E-4D55-4D43-B812-8FF8CB8AA451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE947B5F-85EB-42EC-9ACE-78E14FF67752}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="22380" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Height</t>
   </si>
@@ -74,9 +74,6 @@
     <t>identified gender (male/female/other)</t>
   </si>
   <si>
-    <t>Baggy Pants</t>
-  </si>
-  <si>
     <t>Skinny Jeans</t>
   </si>
   <si>
@@ -111,6 +108,12 @@
   </si>
   <si>
     <t xml:space="preserve">Blue, Black, Silver,Gold  </t>
+  </si>
+  <si>
+    <t>WaistSize</t>
+  </si>
+  <si>
+    <t>BaggyPants</t>
   </si>
 </sst>
 </file>
@@ -172,10 +175,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,16 +443,16 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,13 +463,13 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>180</v>
       </c>
@@ -484,10 +483,10 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>175</v>
       </c>
@@ -501,10 +500,10 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -518,10 +517,10 @@
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>178</v>
       </c>
@@ -535,10 +534,10 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>192</v>
       </c>
@@ -552,10 +551,10 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -569,10 +568,10 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>156</v>
       </c>
@@ -586,10 +585,10 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>166</v>
       </c>
@@ -603,10 +602,10 @@
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>155</v>
       </c>
@@ -620,10 +619,10 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>145</v>
       </c>
@@ -637,10 +636,10 @@
         <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>165</v>
       </c>
@@ -651,10 +650,10 @@
         <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>133</v>
       </c>
@@ -668,10 +667,10 @@
         <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>166</v>
       </c>
@@ -685,10 +684,10 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>154</v>
       </c>
@@ -702,7 +701,7 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -718,14 +717,14 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -736,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -747,7 +746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -758,7 +757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -769,35 +768,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>